<commit_message>
added head classification model
</commit_message>
<xml_diff>
--- a/results/training-history.xlsx
+++ b/results/training-history.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/sc20dzi_leeds_ac_uk/Documents/Year 3/Semester 2/Individual Project/pain-detection-cats/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{5330388D-D83A-6841-9338-8DFE703942D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46A5DD34-5BB3-654A-8F12-58D7FA163189}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{5330388D-D83A-6841-9338-8DFE703942D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82507B05-EA80-6747-A993-533EACA23D1F}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="380" yWindow="500" windowWidth="26780" windowHeight="16940" xr2:uid="{63D227CB-010E-A642-8E82-6251D8EBE2D7}"/>
+    <workbookView minimized="1" xWindow="980" yWindow="560" windowWidth="26780" windowHeight="16940" activeTab="1" xr2:uid="{63D227CB-010E-A642-8E82-6251D8EBE2D7}"/>
   </bookViews>
   <sheets>
     <sheet name="ears" sheetId="1" r:id="rId1"/>
-    <sheet name="eyes" sheetId="2" r:id="rId2"/>
-    <sheet name="muzzle" sheetId="3" r:id="rId3"/>
-    <sheet name="whiskers" sheetId="4" r:id="rId4"/>
+    <sheet name="whiskers" sheetId="4" r:id="rId2"/>
+    <sheet name="eyes" sheetId="2" r:id="rId3"/>
+    <sheet name="muzzle" sheetId="3" r:id="rId4"/>
     <sheet name="head" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="history" localSheetId="0">ears!$A$1:$D$16</definedName>
-    <definedName name="history" localSheetId="1">eyes!$A$1:$D$8</definedName>
-    <definedName name="history" localSheetId="2">muzzle!$A$1:$D$7</definedName>
+    <definedName name="history" localSheetId="2">eyes!$A$1:$D$8</definedName>
+    <definedName name="history" localSheetId="3">muzzle!$A$1:$D$7</definedName>
+    <definedName name="history" localSheetId="1">whiskers!$A$1:$D$17</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -76,11 +77,21 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="4" xr16:uid="{3D5EEE16-47DD-8C44-8086-3E062F470D5E}" name="history3" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/dominika/Library/CloudStorage/OneDrive-UniversityofLeeds/Year 3/Semester 2/Individual Project/pain-detection-cats/results/whiskers/history.csv" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
   <si>
     <t>loss</t>
   </si>
@@ -800,6 +811,617 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>whiskers!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>whiskers!$A$2:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1.3086676597595199</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.04264271259307</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.01226830482482</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0030201673507599</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99493861198425204</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98630684614181496</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97849911451339699</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.95940554141998202</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.941800236701965</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.92151284217834395</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.91534525156021096</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.89227002859115601</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.87130486965179399</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.83338248729705799</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.80774682760238603</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.76073014736175504</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-61F9-5049-9305-2A5ADD50912A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>whiskers!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>whiskers!$B$2:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.36286765336990301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39705884456634499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.41433823108673001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.43014708161353998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.43529412150382901</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.46176472306251498</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.46360296010971003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.48382353782653797</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.49852943420410101</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.52830880880355802</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.53529411554336503</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.54558825492858798</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.57536762952804499</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.604411780834198</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.61911767721176103</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.65220588445663397</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-61F9-5049-9305-2A5ADD50912A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>whiskers!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>val_loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>whiskers!$C$2:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1.01209163665771</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0047851800918499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.00954902172088</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97127091884613004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97106385231018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95706439018249501</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97228813171386697</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96886587142944303</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95914363861083896</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.96670591831207198</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.95380175113677901</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95595848560333196</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.97707325220107999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.97078007459640503</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.96823030710220304</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.975580275058746</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-61F9-5049-9305-2A5ADD50912A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>whiskers!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>val_accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>whiskers!$D$2:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.43318647146224898</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.44346547126769997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.41409692168235701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46696034073829601</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.47283405065536499</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.47577092051505998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.46696034073829601</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.45374450087547302</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.47136563062667802</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.47577092051505998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.48898679018020602</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.46842876076698298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.459618210792541</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.48458150029182401</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.47870779037475503</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.51395004987716597</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-61F9-5049-9305-2A5ADD50912A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1270650128"/>
+        <c:axId val="1270251872"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1270650128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1270251872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1270251872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1270650128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>eyes!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -1248,7 +1870,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -1463,7 +2085,7 @@
                   <c:v>1.17983090877532</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5733858346939</c:v>
+                  <c:v>1.2232879114151001</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.2532879114151001</c:v>
@@ -1859,6 +2481,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2892,6 +3554,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3455,6 +4633,47 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>0</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AF5D36C-6A87-31B1-48BE-7F365DF201CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -3489,7 +4708,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3535,10 +4754,14 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="history" connectionId="4" xr16:uid="{13A063B4-E475-6C45-9629-6750C5201D16}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="history" connectionId="2" xr16:uid="{B0AE7070-FAB0-2344-BF1E-90CA06B0B6B0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="history" connectionId="3" xr16:uid="{F69B5C32-1C52-B645-8F47-124B549AD07A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -3841,7 +5064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12725BF-F493-E145-BBD5-3B0D8E0D1FFD}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
@@ -4081,11 +5304,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BBC5E5-8CBA-CA46-A176-0B3ECF707299}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52EB8990-F52E-6B4A-8A28-31DB22547DBF}">
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="A1:D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="A1:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4109,100 +5332,226 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>5.0219208002090399E-2</v>
+        <v>1.3086676597595199</v>
       </c>
       <c r="B2">
-        <v>0.986292004585266</v>
+        <v>0.36286765336990301</v>
       </c>
       <c r="C2">
-        <v>0.96427881717681796</v>
+        <v>1.01209163665771</v>
       </c>
       <c r="D2">
-        <v>0.72602742910385099</v>
+        <v>0.43318647146224898</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>6.4096160233020699E-2</v>
+        <v>1.04264271259307</v>
       </c>
       <c r="B3">
-        <v>0.98080879449844305</v>
+        <v>0.39705884456634499</v>
       </c>
       <c r="C3">
-        <v>0.82725280523300104</v>
+        <v>1.0047851800918499</v>
       </c>
       <c r="D3">
-        <v>0.72465753555297796</v>
+        <v>0.44346547126769997</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>7.9149343073368003E-2</v>
+        <v>1.01226830482482</v>
       </c>
       <c r="B4">
-        <v>0.97292667627334595</v>
+        <v>0.41433823108673001</v>
       </c>
       <c r="C4">
-        <v>1.0619969367980899</v>
+        <v>1.00954902172088</v>
       </c>
       <c r="D4">
-        <v>0.72602742910385099</v>
+        <v>0.41409692168235701</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3.9371091872453599E-2</v>
+        <v>1.0030201673507599</v>
       </c>
       <c r="B5">
-        <v>0.986977398395538</v>
+        <v>0.43014708161353998</v>
       </c>
       <c r="C5">
-        <v>1.09598660469055</v>
+        <v>0.97127091884613004</v>
       </c>
       <c r="D5">
-        <v>0.73287671804428101</v>
+        <v>0.46696034073829601</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>9.86689794808626E-3</v>
+        <v>0.99493861198425204</v>
       </c>
       <c r="B6">
-        <v>0.99760109186172397</v>
+        <v>0.43529412150382901</v>
       </c>
       <c r="C6">
-        <v>1.3891570568084699</v>
+        <v>0.97106385231018</v>
       </c>
       <c r="D6">
-        <v>0.709589064121246</v>
+        <v>0.47283405065536499</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1.6789935529232001E-2</v>
+        <v>0.98630684614181496</v>
       </c>
       <c r="B7">
-        <v>0.99520218372344904</v>
+        <v>0.46176472306251498</v>
       </c>
       <c r="C7">
-        <v>1.1107751131057699</v>
+        <v>0.95706439018249501</v>
       </c>
       <c r="D7">
-        <v>0.71917808055877597</v>
+        <v>0.47577092051505998</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2.2421741858124698E-2</v>
+        <v>0.97849911451339699</v>
       </c>
       <c r="B8">
-        <v>0.99417412281036299</v>
+        <v>0.46360296010971003</v>
       </c>
       <c r="C8">
-        <v>1.1668959856033301</v>
+        <v>0.97228813171386697</v>
       </c>
       <c r="D8">
-        <v>0.72602742910385099</v>
+        <v>0.46696034073829601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0.95940554141998202</v>
+      </c>
+      <c r="B9">
+        <v>0.48382353782653797</v>
+      </c>
+      <c r="C9">
+        <v>0.96886587142944303</v>
+      </c>
+      <c r="D9">
+        <v>0.45374450087547302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0.941800236701965</v>
+      </c>
+      <c r="B10">
+        <v>0.49852943420410101</v>
+      </c>
+      <c r="C10">
+        <v>0.95914363861083896</v>
+      </c>
+      <c r="D10">
+        <v>0.47136563062667802</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0.92151284217834395</v>
+      </c>
+      <c r="B11">
+        <v>0.52830880880355802</v>
+      </c>
+      <c r="C11">
+        <v>0.96670591831207198</v>
+      </c>
+      <c r="D11">
+        <v>0.47577092051505998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.91534525156021096</v>
+      </c>
+      <c r="B12">
+        <v>0.53529411554336503</v>
+      </c>
+      <c r="C12">
+        <v>0.95380175113677901</v>
+      </c>
+      <c r="D12">
+        <v>0.48898679018020602</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0.89227002859115601</v>
+      </c>
+      <c r="B13">
+        <v>0.54558825492858798</v>
+      </c>
+      <c r="C13">
+        <v>0.95595848560333196</v>
+      </c>
+      <c r="D13">
+        <v>0.46842876076698298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>0.87130486965179399</v>
+      </c>
+      <c r="B14">
+        <v>0.57536762952804499</v>
+      </c>
+      <c r="C14">
+        <v>0.97707325220107999</v>
+      </c>
+      <c r="D14">
+        <v>0.459618210792541</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0.83338248729705799</v>
+      </c>
+      <c r="B15">
+        <v>0.604411780834198</v>
+      </c>
+      <c r="C15">
+        <v>0.97078007459640503</v>
+      </c>
+      <c r="D15">
+        <v>0.48458150029182401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>0.80774682760238603</v>
+      </c>
+      <c r="B16">
+        <v>0.61911767721176103</v>
+      </c>
+      <c r="C16">
+        <v>0.96823030710220304</v>
+      </c>
+      <c r="D16">
+        <v>0.47870779037475503</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0.76073014736175504</v>
+      </c>
+      <c r="B17">
+        <v>0.65220588445663397</v>
+      </c>
+      <c r="C17">
+        <v>0.975580275058746</v>
+      </c>
+      <c r="D17">
+        <v>0.51395004987716597</v>
       </c>
     </row>
   </sheetData>
@@ -4212,11 +5561,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3CEF92-3CA7-7B43-899B-0DF1D46E9F0A}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BBC5E5-8CBA-CA46-A176-0B3ECF707299}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4240,86 +5589,100 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0.61367881298065097</v>
+        <v>5.0219208002090399E-2</v>
       </c>
       <c r="B2">
-        <v>0.727114498615264</v>
+        <v>0.986292004585266</v>
       </c>
       <c r="C2">
-        <v>1.0735671520233101</v>
+        <v>0.96427881717681796</v>
       </c>
       <c r="D2">
-        <v>0.47426983714103699</v>
+        <v>0.72602742910385099</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>0.55221807956695501</v>
+        <v>6.4096160233020699E-2</v>
       </c>
       <c r="B3">
-        <v>0.76226937770843495</v>
+        <v>0.98080879449844305</v>
       </c>
       <c r="C3">
-        <v>1.1899781227111801</v>
+        <v>0.82725280523300104</v>
       </c>
       <c r="D3">
-        <v>0.45897078514099099</v>
+        <v>0.72465753555297796</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>0.53416734933853105</v>
+        <v>7.9149343073368003E-2</v>
       </c>
       <c r="B4">
-        <v>0.77514791488647405</v>
+        <v>0.97292667627334595</v>
       </c>
       <c r="C4">
-        <v>1.12306892871856</v>
+        <v>1.0619969367980899</v>
       </c>
       <c r="D4">
-        <v>0.46036162972450201</v>
+        <v>0.72602742910385099</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>0.48876467347144997</v>
+        <v>3.9371091872453599E-2</v>
       </c>
       <c r="B5">
-        <v>0.79324746131896895</v>
+        <v>0.986977398395538</v>
       </c>
       <c r="C5">
-        <v>1.17983090877532</v>
+        <v>1.09598660469055</v>
       </c>
       <c r="D5">
-        <v>0.47983309626579201</v>
+        <v>0.73287671804428101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>0.464827209711074</v>
+        <v>9.86689794808626E-3</v>
       </c>
       <c r="B6">
-        <v>0.80717021226882901</v>
+        <v>0.99760109186172397</v>
       </c>
       <c r="C6">
-        <v>1.5733858346939</v>
+        <v>1.3891570568084699</v>
       </c>
       <c r="D6">
-        <v>0.44506257772445601</v>
+        <v>0.709589064121246</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>0.43481814861297602</v>
+        <v>1.6789935529232001E-2</v>
       </c>
       <c r="B7">
-        <v>0.82352942228317205</v>
+        <v>0.99520218372344904</v>
       </c>
       <c r="C7">
-        <v>1.2532879114151001</v>
+        <v>1.1107751131057699</v>
       </c>
       <c r="D7">
-        <v>0.49235048890113797</v>
+        <v>0.71917808055877597</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2.2421741858124698E-2</v>
+      </c>
+      <c r="B8">
+        <v>0.99417412281036299</v>
+      </c>
+      <c r="C8">
+        <v>1.1668959856033301</v>
+      </c>
+      <c r="D8">
+        <v>0.72602742910385099</v>
       </c>
     </row>
   </sheetData>
@@ -4329,14 +5692,119 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52EB8990-F52E-6B4A-8A28-31DB22547DBF}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3CEF92-3CA7-7B43-899B-0DF1D46E9F0A}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.61367881298065097</v>
+      </c>
+      <c r="B2">
+        <v>0.727114498615264</v>
+      </c>
+      <c r="C2">
+        <v>1.0735671520233101</v>
+      </c>
+      <c r="D2">
+        <v>0.47426983714103699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.55221807956695501</v>
+      </c>
+      <c r="B3">
+        <v>0.76226937770843495</v>
+      </c>
+      <c r="C3">
+        <v>1.1899781227111801</v>
+      </c>
+      <c r="D3">
+        <v>0.45897078514099099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.53416734933853105</v>
+      </c>
+      <c r="B4">
+        <v>0.77514791488647405</v>
+      </c>
+      <c r="C4">
+        <v>1.12306892871856</v>
+      </c>
+      <c r="D4">
+        <v>0.46036162972450201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.48876467347144997</v>
+      </c>
+      <c r="B5">
+        <v>0.79324746131896895</v>
+      </c>
+      <c r="C5">
+        <v>1.17983090877532</v>
+      </c>
+      <c r="D5">
+        <v>0.47983309626579201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0.464827209711074</v>
+      </c>
+      <c r="B6">
+        <v>0.80717021226882901</v>
+      </c>
+      <c r="C6">
+        <v>1.2232879114151001</v>
+      </c>
+      <c r="D6">
+        <v>0.44506257772445601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.43481814861297602</v>
+      </c>
+      <c r="B7">
+        <v>0.82352942228317205</v>
+      </c>
+      <c r="C7">
+        <v>1.2532879114151001</v>
+      </c>
+      <c r="D7">
+        <v>0.49235048890113797</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>